<commit_message>
kpis set for brand
</commit_message>
<xml_diff>
--- a/Projects/GMIUS/Data/GMIUS Template v0.1.xlsx
+++ b/Projects/GMIUS/Data/GMIUS Template v0.1.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="KPIs" sheetId="1" state="visible" r:id="rId2"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="16">
   <si>
     <t xml:space="preserve">KPI Name</t>
   </si>
@@ -47,7 +47,7 @@
     <t xml:space="preserve">Session Level</t>
   </si>
   <si>
-    <t xml:space="preserve">Channel Aggregation SOS</t>
+    <t xml:space="preserve">Brand Aggregation SOS</t>
   </si>
   <si>
     <t xml:space="preserve">Aggregation</t>
@@ -59,16 +59,7 @@
     <t xml:space="preserve">Y</t>
   </si>
   <si>
-    <t xml:space="preserve">Channel Aggregation Linear SOS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Retailer Aggregation SOS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Retailer Aggregation Linear SOS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Aggregation Level</t>
+    <t xml:space="preserve">Brand Aggregation Linear SOS</t>
   </si>
   <si>
     <t xml:space="preserve">SOS Type</t>
@@ -78,9 +69,6 @@
   </si>
   <si>
     <t xml:space="preserve">Linear SOS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Retailer</t>
   </si>
 </sst>
 </file>
@@ -95,6 +83,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -154,12 +143,8 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -180,20 +165,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H30"/>
+  <dimension ref="A1:H27"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="28.2040816326531"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="15.9744897959184"/>
-    <col collapsed="false" hidden="false" max="7" min="5" style="0" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="15"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="27.5408163265306"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="15.6581632653061"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="14.4438775510204"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -223,7 +205,7 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="0" t="s">
         <v>8</v>
       </c>
       <c r="B2" s="0" t="s">
@@ -237,7 +219,7 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="0" t="s">
         <v>12</v>
       </c>
       <c r="B3" s="0" t="s">
@@ -250,37 +232,12 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B4" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" s="0" t="s">
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="0" t="s">
         <v>10</v>
       </c>
-      <c r="H4" s="0" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B5" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="H5" s="0" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="0" t="s">
-        <v>10</v>
+      <c r="B27" s="0" t="s">
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -299,17 +256,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B9" activeCellId="0" sqref="B9"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="27.5102040816327"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.0204081632653"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="26.8622448979592"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -317,10 +272,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="C1" s="0" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -328,10 +280,7 @@
         <v>8</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" s="0" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -339,38 +288,13 @@
         <v>12</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" s="0" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C4" s="0" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="B5" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="C5" s="0" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>